<commit_message>
Completed Italian - English translation.
</commit_message>
<xml_diff>
--- a/Assets/Texts/itaEn.xlsx
+++ b/Assets/Texts/itaEn.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="419">
   <si>
     <t>Key</t>
   </si>
@@ -698,9 +698,6 @@
     <t>Hi, what is this debris?</t>
   </si>
   <si>
-    <t>Its what remains of my spaceship that crashed here.{w=3}{c}{w=3}Unfortunately the power oil got dispersed, so I'm blocked here.{c}To progress I need three oil flasks.</t>
-  </si>
-  <si>
     <t>I'm ready to help!</t>
   </si>
   <si>
@@ -722,9 +719,6 @@
     <t>I have one flask.</t>
   </si>
   <si>
-    <t>Its a good start. Find more please.</t>
-  </si>
-  <si>
     <t>I have two flasks. Only one missing!</t>
   </si>
   <si>
@@ -734,12 +728,6 @@
     <t>Thank, thanks a lot!</t>
   </si>
   <si>
-    <t>Take this tool: its an "Italian adjustable spanner"</t>
-  </si>
-  <si>
-    <t>I found a map of the island!\nI can open it and close it by clicking its icon</t>
-  </si>
-  <si>
     <t>We can fix the portal with the Italian spanner.</t>
   </si>
   <si>
@@ -767,9 +755,6 @@
     <t>YOU WON!{w}</t>
   </si>
   <si>
-    <t>I suspect that its not the right code...</t>
-  </si>
-  <si>
     <t>So cold!</t>
   </si>
   <si>
@@ -782,9 +767,6 @@
     <t>This ice cave seems so sold, but wth Malik's fur coat I can make it.</t>
   </si>
   <si>
-    <t>I can't enter that ice cave: its too cold!</t>
-  </si>
-  <si>
     <t>Where are you running? You didn't find my shovel!</t>
   </si>
   <si>
@@ -794,27 +776,15 @@
     <t>I collected Fluffi's oil in a flask!</t>
   </si>
   <si>
-    <t>Who are you? Its so nice to meet a person after such a long time.{w=2}{c}Finally I can tell my story to someone.</t>
-  </si>
-  <si>
     <t>I'm here to listen.</t>
   </si>
   <si>
-    <t>Great! I'm a scientist called barni and I've invented a machine that can take you from one dimension to another.{w=6}{c}But it broke so I was blocked here, but I'd like to get back home with my friend Fluffi.{w=5}{c}Wait a second, can you find my shovel, its in this room.</t>
-  </si>
-  <si>
     <t>I'm not interested.</t>
   </si>
   <si>
     <t>Well you'll have to listen, otherwise I won't let you out!</t>
   </si>
   <si>
-    <t>Come on, find my shovel! Its impossible to see it in the dark, but its here! Look carefully.</t>
-  </si>
-  <si>
-    <t>Thank you! I will start immediately repairing the bridge.{w=3}{c}If you'll ask Fluffi it will give you some oil:  it secretes it from its fluffish flufficols.</t>
-  </si>
-  <si>
     <t>Without his diary Trevor the magician won't remember a thing.</t>
   </si>
   <si>
@@ -1034,12 +1004,6 @@
     <t>I'll reward you after you will have given me oil.</t>
   </si>
   <si>
-    <t>its not a toast - unfortunately - its Malik's fur.</t>
-  </si>
-  <si>
-    <t>Its betten not to season salad with this oil.</t>
-  </si>
-  <si>
     <t>The selfish - ops elfish medicine.</t>
   </si>
   <si>
@@ -1049,9 +1013,6 @@
     <t>Remember that you'll die one day!\nbut not in this game.</t>
   </si>
   <si>
-    <t>A diary... I can't read it though as its not my diary.</t>
-  </si>
-  <si>
     <t>A spanner... an Italian one.</t>
   </si>
   <si>
@@ -1061,9 +1022,6 @@
     <t>I found a pet dragon! So nice.</t>
   </si>
   <si>
-    <t>The portal seems broken! I need some toos!{w=3}\nA British spanner? Or even from some other country!</t>
-  </si>
-  <si>
     <t>Ok so now the portal is fixed, what is now missing is just the activation code.</t>
   </si>
   <si>
@@ -1088,12 +1046,6 @@
     <t>OK, I will help you!</t>
   </si>
   <si>
-    <t>Now Trevo the magician is happy.</t>
-  </si>
-  <si>
-    <t>I have Trevor's diary!{w}\nHe lost diary and memory fighting demons in the undergrund.</t>
-  </si>
-  <si>
     <t>Ah! Now I remember!{w}\nThank you, now I can help you: ask me for something and I will get it for you.</t>
   </si>
   <si>
@@ -1112,15 +1064,9 @@
     <t>There you go.</t>
   </si>
   <si>
-    <t>Linzi is still desperate. We should estinguish the lava.</t>
-  </si>
-  <si>
     <t>What happened here? Why is there lava everywhere?</t>
   </si>
   <si>
-    <t>Sigh… sigh… I'm Linzi the elf.{w}\nThe vulcano exploded and my house is on fire!</t>
-  </si>
-  <si>
     <t>And what can we do?</t>
   </si>
   <si>
@@ -1142,9 +1088,6 @@
     <t xml:space="preserve">Mago Trevor portrait_mago_happy </t>
   </si>
   <si>
-    <t>The only thing that can estinguish lava is water,{w=2}but I'm too upset to go look for it... sigh… sigh…</t>
-  </si>
-  <si>
     <t>I can help you!</t>
   </si>
   <si>
@@ -1166,12 +1109,6 @@
     <t>...</t>
   </si>
   <si>
-    <t>I don't have the strenght to divert the river and extinguish the lava...</t>
-  </si>
-  <si>
-    <t>Done! I diverted the river and the lava is almost exhaused.</t>
-  </si>
-  <si>
     <t>Hurray!{w}\nI looked everywhere, but the only good thing remaining is this medicine. Take it.</t>
   </si>
   <si>
@@ -1202,9 +1139,6 @@
     <t>I'll take you out of here.</t>
   </si>
   <si>
-    <t>I'll get you out of here in exchenge of something.</t>
-  </si>
-  <si>
     <t>I will give you a prize in the future... After we got out...</t>
   </si>
   <si>
@@ -1218,6 +1152,144 @@
   </si>
   <si>
     <t>Why are you suffering?</t>
+  </si>
+  <si>
+    <t>I was wounded while hunting, help me and I will give you three important life advices!</t>
+  </si>
+  <si>
+    <t>You intrigued me, what do you need?</t>
+  </si>
+  <si>
+    <t>I need a medicine.</t>
+  </si>
+  <si>
+    <t>I have an elvish medicine. Take it.</t>
+  </si>
+  <si>
+    <t>You still want t listen to my wise advice?</t>
+  </si>
+  <si>
+    <t>Here are my life advices: drink a lot when you are thirsty...{w}\n…eat a lot when you are hungry…{w}{c}… and breath deeply when you need to breathe.</t>
+  </si>
+  <si>
+    <t>Ah... Thank you. Ok, I go now...</t>
+  </si>
+  <si>
+    <t>Could you lend me your fur?</t>
+  </si>
+  <si>
+    <t>have pity on me, I'm ill!{w}\nAt least leave me the fur to protect myself from fever.</t>
+  </si>
+  <si>
+    <t>Sure! Now that I recovered I don't need it anymore.</t>
+  </si>
+  <si>
+    <t>Bzz… hi!{w}\nI'm Zot the android and I feel so lonely..{w=3}\nCan I become your friend?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Bzz... please!</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>Zot The Android</t>
+  </si>
+  <si>
+    <t>Quby The Robot</t>
+  </si>
+  <si>
+    <t>Malik The Native</t>
+  </si>
+  <si>
+    <t>Trevor The Magician</t>
+  </si>
+  <si>
+    <t>Linzi The Elf</t>
+  </si>
+  <si>
+    <t>Barni The Scientist</t>
+  </si>
+  <si>
+    <t>I beieve this is not the right code...</t>
+  </si>
+  <si>
+    <t>Bzz… thanks!{w}\nIn exchange I am available for dangerous missions.</t>
+  </si>
+  <si>
+    <t>Hmm. Then you are coming with me? Cool...</t>
+  </si>
+  <si>
+    <t>This is the beginning of our story…{w} \nHow did we end on this beach?{w} Are we alone?{w}\nMost of al…{w} {color=red}how will we get out of here?{/color}</t>
+  </si>
+  <si>
+    <t>It's what remains of my spaceship that crashed here.{w=3}{c}{w=3}Unfortunately the power oil got dispersed, so I'm blocked here.{c}To progress I need three oil flasks.</t>
+  </si>
+  <si>
+    <t>It's a good start. Find more please.</t>
+  </si>
+  <si>
+    <t>Take this tool: it's an "Italian adjustable spanner"</t>
+  </si>
+  <si>
+    <t>It's better not to season salad with this oil.</t>
+  </si>
+  <si>
+    <t>The portal seems broken! I need some tools!{w=3}\nA British spanner? Or even from some other country!</t>
+  </si>
+  <si>
+    <t>I found a map of the island!\nI can open it and close it by clicking it's icon</t>
+  </si>
+  <si>
+    <t>it's not a toast - unfortunately - it's Malik's fur.</t>
+  </si>
+  <si>
+    <t>A diary... I can't read it though as it's not my diary.</t>
+  </si>
+  <si>
+    <t>I suspect that it's not the right code...</t>
+  </si>
+  <si>
+    <t>I can't enter that ice cave: it's too cold!</t>
+  </si>
+  <si>
+    <t>Who are you? it's so nice to meet a person after such a long time.{w=2}{c}Finally I can tell my story to someone.</t>
+  </si>
+  <si>
+    <t>Great! I'm a scientist called barni and I've invented a machine that can take you from one dimension to another.{w=6}{c}But it broke so I was blocked here, but I'd like to get back home with my friend Fluffi.{w=5}{c}Wait a second, can you find my shovel, it's in this room.</t>
+  </si>
+  <si>
+    <t>Come on, find my shovel! it's impossible to see it in the dark, but it's here! Look carefully.</t>
+  </si>
+  <si>
+    <t>Thank you! I will start immediately repairing the bridge.{w=3}{c}If you'll ask Fluffi it will give you some oil:  it secretes it from it's fluffish flufficols.</t>
+  </si>
+  <si>
+    <t>Now Trevor the magician is happy.</t>
+  </si>
+  <si>
+    <t>I have Trevor's diary!{w}\nHe lost diary and memory fighting demons in the underground.</t>
+  </si>
+  <si>
+    <t>Linzi is still desperate. We should extinguish the lava.</t>
+  </si>
+  <si>
+    <t>The only thing that can extinguish lava is water,{w=2}but I'm too upset to go look for it... sigh… sigh…</t>
+  </si>
+  <si>
+    <t>Sigh… sigh… I'm Linzi the elf.{w}\nThe volcano exploded and my house is on fire!</t>
+  </si>
+  <si>
+    <t>I don't have the strength to divert the river and extinguish the lava...</t>
+  </si>
+  <si>
+    <t>Done! I diverted the river and the lava is almost exhausted.</t>
+  </si>
+  <si>
+    <t>I'll get you out of here in exchange of something.</t>
   </si>
 </sst>
 </file>
@@ -1561,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B105" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.7109375" defaultRowHeight="61.5" customHeight="1"/>
@@ -1638,10 +1710,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>221</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="61.5" customHeight="1">
@@ -1652,7 +1724,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="61.5" customHeight="1">
@@ -1663,7 +1735,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="61.5" customHeight="1">
@@ -1677,7 +1749,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="61.5" customHeight="1">
@@ -1691,7 +1763,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="61.5" customHeight="1">
@@ -1702,10 +1774,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="61.5" customHeight="1">
@@ -1719,7 +1791,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="61.5" customHeight="1">
@@ -1730,10 +1802,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="61.5" customHeight="1">
@@ -1747,7 +1819,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="61.5" customHeight="1">
@@ -1758,10 +1830,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>229</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="61.5" customHeight="1">
@@ -1772,10 +1844,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="61.5" customHeight="1">
@@ -1789,7 +1861,7 @@
         <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="61.5" customHeight="1">
@@ -1803,7 +1875,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="61.5" customHeight="1">
@@ -1814,10 +1886,10 @@
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>233</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="61.5" customHeight="1">
@@ -1828,10 +1900,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>234</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="61.5" customHeight="1">
@@ -1842,10 +1914,10 @@
         <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>333</v>
+        <v>403</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="61.5" customHeight="1">
@@ -1856,10 +1928,10 @@
         <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>334</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="61.5" customHeight="1">
@@ -1870,10 +1942,10 @@
         <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="61.5" customHeight="1">
@@ -1884,10 +1956,10 @@
         <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="61.5" customHeight="1">
@@ -1898,10 +1970,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="61.5" customHeight="1">
@@ -1912,10 +1984,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>338</v>
+        <v>404</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="61.5" customHeight="1">
@@ -1926,10 +1998,10 @@
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="61.5" customHeight="1">
@@ -1940,10 +2012,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="61.5" customHeight="1">
@@ -1954,10 +2026,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="61.5" customHeight="1">
@@ -1971,7 +2043,7 @@
         <v>48</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="61.5" customHeight="1">
@@ -1982,10 +2054,10 @@
         <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>342</v>
+        <v>401</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="61.5" customHeight="1">
@@ -1996,10 +2068,10 @@
         <v>4</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="61.5" customHeight="1">
@@ -2010,10 +2082,10 @@
         <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="61.5" customHeight="1">
@@ -2043,10 +2115,10 @@
         <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="61.5" customHeight="1">
@@ -2060,7 +2132,7 @@
         <v>57</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="61.5" customHeight="1">
@@ -2071,10 +2143,10 @@
         <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="61.5" customHeight="1">
@@ -2085,10 +2157,10 @@
         <v>179</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="61.5" customHeight="1">
@@ -2099,10 +2171,10 @@
         <v>42</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="61.5" customHeight="1">
@@ -2113,10 +2185,10 @@
         <v>75</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="61.5" customHeight="1">
@@ -2124,13 +2196,13 @@
         <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="61.5" customHeight="1">
@@ -2141,10 +2213,10 @@
         <v>131</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="61.5" customHeight="1">
@@ -2152,13 +2224,13 @@
         <v>64</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="61.5" customHeight="1">
@@ -2169,46 +2241,46 @@
         <v>66</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="61.5" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>244</v>
+        <v>405</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="61.5" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="61.5" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="61.5" customHeight="1">
@@ -2222,7 +2294,7 @@
         <v>68</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="61.5" customHeight="1">
@@ -2233,10 +2305,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="61.5" customHeight="1">
@@ -2247,10 +2319,10 @@
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="61.5" customHeight="1">
@@ -2264,7 +2336,7 @@
         <v>72</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="61.5" customHeight="1">
@@ -2275,10 +2347,10 @@
         <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>249</v>
+        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="61.5" customHeight="1">
@@ -2292,7 +2364,7 @@
         <v>76</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="61.5" customHeight="1">
@@ -2306,7 +2378,7 @@
         <v>78</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="61.5" customHeight="1">
@@ -2320,7 +2392,7 @@
         <v>80</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="61.5" customHeight="1">
@@ -2334,7 +2406,7 @@
         <v>82</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>253</v>
+        <v>407</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="61.5" customHeight="1">
@@ -2348,7 +2420,7 @@
         <v>84</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="61.5" customHeight="1">
@@ -2359,10 +2431,10 @@
         <v>75</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>255</v>
+        <v>408</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="61.5" customHeight="1">
@@ -2376,7 +2448,7 @@
         <v>87</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="61.5" customHeight="1">
@@ -2390,7 +2462,7 @@
         <v>90</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="61.5" customHeight="1">
@@ -2401,10 +2473,10 @@
         <v>75</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>258</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="61.5" customHeight="1">
@@ -2415,10 +2487,10 @@
         <v>75</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>259</v>
+        <v>410</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="61.5" customHeight="1">
@@ -2429,10 +2501,10 @@
         <v>4</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="61.5" customHeight="1">
@@ -2443,10 +2515,10 @@
         <v>95</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="61.5" customHeight="1">
@@ -2457,10 +2529,10 @@
         <v>4</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="61.5" customHeight="1">
@@ -2474,7 +2546,7 @@
         <v>98</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="61.5" customHeight="1">
@@ -2488,7 +2560,7 @@
         <v>100</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="61.5" customHeight="1">
@@ -2499,10 +2571,10 @@
         <v>95</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="61.5" customHeight="1">
@@ -2513,10 +2585,10 @@
         <v>4</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="61.5" customHeight="1">
@@ -2527,10 +2599,10 @@
         <v>35</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>351</v>
+        <v>411</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="61.5" customHeight="1">
@@ -2544,7 +2616,7 @@
         <v>105</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>352</v>
+        <v>412</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="61.5" customHeight="1">
@@ -2555,10 +2627,10 @@
         <v>107</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="61.5" customHeight="1">
@@ -2569,7 +2641,7 @@
         <v>109</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="61.5" customHeight="1">
@@ -2580,7 +2652,7 @@
         <v>111</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="61.5" customHeight="1">
@@ -2594,7 +2666,7 @@
         <v>113</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="61.5" customHeight="1">
@@ -2608,7 +2680,7 @@
         <v>115</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="61.5" customHeight="1">
@@ -2622,7 +2694,7 @@
         <v>117</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="61.5" customHeight="1">
@@ -2633,10 +2705,10 @@
         <v>66</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>359</v>
+        <v>413</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="61.5" customHeight="1">
@@ -2647,10 +2719,10 @@
         <v>120</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="61.5" customHeight="1">
@@ -2661,10 +2733,10 @@
         <v>122</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>361</v>
+        <v>415</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="61.5" customHeight="1">
@@ -2678,7 +2750,7 @@
         <v>124</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="61.5" customHeight="1">
@@ -2689,10 +2761,10 @@
         <v>122</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>369</v>
+        <v>414</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="61.5" customHeight="1">
@@ -2703,7 +2775,7 @@
         <v>127</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="61.5" customHeight="1">
@@ -2714,7 +2786,7 @@
         <v>129</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="61.5" customHeight="1">
@@ -2725,10 +2797,10 @@
         <v>131</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="61.5" customHeight="1">
@@ -2739,10 +2811,10 @@
         <v>133</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="61.5" customHeight="1">
@@ -2753,10 +2825,10 @@
         <v>4</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="61.5" customHeight="1">
@@ -2767,10 +2839,10 @@
         <v>66</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>377</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="61.5" customHeight="1">
@@ -2784,7 +2856,7 @@
         <v>137</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="61.5" customHeight="1">
@@ -2795,10 +2867,10 @@
         <v>40</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="61.5" customHeight="1">
@@ -2812,7 +2884,7 @@
         <v>140</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>378</v>
+        <v>417</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="61.5" customHeight="1">
@@ -2823,10 +2895,10 @@
         <v>131</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="61.5" customHeight="1">
@@ -2840,7 +2912,7 @@
         <v>143</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="61.5" customHeight="1">
@@ -2854,7 +2926,7 @@
         <v>145</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="61.5" customHeight="1">
@@ -2865,10 +2937,10 @@
         <v>4</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="61.5" customHeight="1">
@@ -2879,10 +2951,10 @@
         <v>4</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="61.5" customHeight="1">
@@ -2896,7 +2968,7 @@
         <v>149</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="61.5" customHeight="1">
@@ -2907,10 +2979,10 @@
         <v>42</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="61.5" customHeight="1">
@@ -2924,7 +2996,7 @@
         <v>152</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="61.5" customHeight="1">
@@ -2935,10 +3007,10 @@
         <v>154</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="61.5" customHeight="1">
@@ -2949,10 +3021,10 @@
         <v>42</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="61.5" customHeight="1">
@@ -2960,10 +3032,10 @@
         <v>156</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="61.5" customHeight="1">
@@ -2971,10 +3043,10 @@
         <v>157</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>389</v>
+        <v>418</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="61.5" customHeight="1">
@@ -2985,10 +3057,10 @@
         <v>42</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="61.5" customHeight="1">
@@ -3002,7 +3074,7 @@
         <v>161</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="61.5" customHeight="1">
@@ -3013,10 +3085,10 @@
         <v>35</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="61.5" customHeight="1">
@@ -3030,7 +3102,7 @@
         <v>165</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="61.5" customHeight="1">
@@ -3041,10 +3113,10 @@
         <v>4</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="61.5" customHeight="1">
@@ -3055,7 +3127,10 @@
         <v>164</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>323</v>
+        <v>313</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="61.5" customHeight="1">
@@ -3068,6 +3143,9 @@
       <c r="C110" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="D110" s="1" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="111" spans="1:4" ht="61.5" customHeight="1">
       <c r="A111" s="2" t="s">
@@ -3079,6 +3157,9 @@
       <c r="C111" s="1" t="s">
         <v>171</v>
       </c>
+      <c r="D111" s="1" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="112" spans="1:4" ht="61.5" customHeight="1">
       <c r="A112" s="2" t="s">
@@ -3090,8 +3171,11 @@
       <c r="C112" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D112" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="61.5" customHeight="1">
       <c r="A113" s="2" t="s">
         <v>174</v>
       </c>
@@ -3101,8 +3185,11 @@
       <c r="C113" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D113" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="61.5" customHeight="1">
       <c r="A114" s="2" t="s">
         <v>176</v>
       </c>
@@ -3112,8 +3199,11 @@
       <c r="C114" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D114" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="61.5" customHeight="1">
       <c r="A115" s="2" t="s">
         <v>178</v>
       </c>
@@ -3121,10 +3211,13 @@
         <v>179</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="61.5" customHeight="1">
+        <v>314</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="61.5" customHeight="1">
       <c r="A116" s="2" t="s">
         <v>180</v>
       </c>
@@ -3132,10 +3225,13 @@
         <v>120</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="61.5" customHeight="1">
+        <v>315</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="61.5" customHeight="1">
       <c r="A117" s="2" t="s">
         <v>181</v>
       </c>
@@ -3143,10 +3239,13 @@
         <v>4</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="61.5" customHeight="1">
+        <v>316</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="61.5" customHeight="1">
       <c r="A118" s="2" t="s">
         <v>182</v>
       </c>
@@ -3156,8 +3255,11 @@
       <c r="C118" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D118" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="61.5" customHeight="1">
       <c r="A119" s="2" t="s">
         <v>184</v>
       </c>
@@ -3167,8 +3269,11 @@
       <c r="C119" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D119" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="61.5" customHeight="1">
       <c r="A120" s="2" t="s">
         <v>186</v>
       </c>
@@ -3176,26 +3281,35 @@
         <v>187</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="61.5" customHeight="1">
+        <v>317</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="61.5" customHeight="1">
       <c r="A121" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D121" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="61.5" customHeight="1">
       <c r="A122" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D122" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="61.5" customHeight="1">
       <c r="A123" s="2" t="s">
         <v>192</v>
       </c>
@@ -3205,8 +3319,11 @@
       <c r="C123" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D123" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="61.5" customHeight="1">
       <c r="A124" s="2" t="s">
         <v>194</v>
       </c>
@@ -3214,10 +3331,13 @@
         <v>187</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="61.5" customHeight="1">
+        <v>318</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="61.5" customHeight="1">
       <c r="A125" s="2" t="s">
         <v>195</v>
       </c>
@@ -3227,8 +3347,11 @@
       <c r="C125" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D125" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="61.5" customHeight="1">
       <c r="A126" s="2" t="s">
         <v>197</v>
       </c>
@@ -3236,10 +3359,13 @@
         <v>4</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="61.5" customHeight="1">
+        <v>311</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="61.5" customHeight="1">
       <c r="A127" s="2" t="s">
         <v>198</v>
       </c>
@@ -3247,10 +3373,13 @@
         <v>22</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="61.5" customHeight="1">
+        <v>319</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="61.5" customHeight="1">
       <c r="A128" s="2" t="s">
         <v>199</v>
       </c>
@@ -3258,29 +3387,38 @@
         <v>35</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="61.5" customHeight="1">
+        <v>320</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="61.5" customHeight="1">
       <c r="A129" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="61.5" customHeight="1">
+        <v>321</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="61.5" customHeight="1">
       <c r="A130" s="2" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="61.5" customHeight="1">
+        <v>276</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="61.5" customHeight="1">
       <c r="A131" s="2" t="s">
         <v>201</v>
       </c>
@@ -3290,8 +3428,11 @@
       <c r="C131" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D131" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="61.5" customHeight="1">
       <c r="A132" s="2" t="s">
         <v>203</v>
       </c>
@@ -3301,8 +3442,11 @@
       <c r="C132" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D132" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="61.5" customHeight="1">
       <c r="A133" s="2" t="s">
         <v>205</v>
       </c>
@@ -3312,8 +3456,11 @@
       <c r="C133" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D133" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="61.5" customHeight="1">
       <c r="A134" s="2" t="s">
         <v>207</v>
       </c>
@@ -3323,8 +3470,11 @@
       <c r="C134" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D134" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="61.5" customHeight="1">
       <c r="A135" s="2" t="s">
         <v>209</v>
       </c>
@@ -3334,8 +3484,11 @@
       <c r="C135" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D135" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="61.5" customHeight="1">
       <c r="A136" s="2" t="s">
         <v>211</v>
       </c>
@@ -3345,8 +3498,11 @@
       <c r="C136" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D136" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="61.5" customHeight="1">
       <c r="A137" s="2" t="s">
         <v>213</v>
       </c>
@@ -3356,8 +3512,11 @@
       <c r="C137" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="61.5" customHeight="1">
+      <c r="D137" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="61.5" customHeight="1">
       <c r="A138" s="2" t="s">
         <v>215</v>
       </c>
@@ -3366,6 +3525,9 @@
       </c>
       <c r="C138" s="1" t="s">
         <v>216</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>